<commit_message>
It's a Welch test
turns out that the Welch test (right-tailed T-test for unequal variance) is the equivalent test statistics
</commit_message>
<xml_diff>
--- a/compute p-value.xlsx
+++ b/compute p-value.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>mu</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>p-value</t>
+  </si>
+  <si>
+    <t>Welch-Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T </t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -80,7 +89,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -88,15 +97,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,11 +454,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D267"/>
+  <dimension ref="A2:G267"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6150" ySplit="7200" topLeftCell="G257"/>
-      <selection activeCell="C5" sqref="C5"/>
+      <pane xSplit="9930" ySplit="7200" topLeftCell="G257"/>
+      <selection activeCell="G7" sqref="G7"/>
       <selection pane="topRight" activeCell="J5" sqref="J5"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="J10" activeCellId="1" sqref="G10:G269 J10:J269"/>
@@ -392,7 +469,7 @@
     <col min="2" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -400,7 +477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -410,8 +487,12 @@
       <c r="C3" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -421,8 +502,15 @@
       <c r="C4" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="7">
+        <f>(C3-B3)/(SQRT(B4^2+C4^2))</f>
+        <v>1.4142135623730949</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
@@ -430,8 +518,15 @@
         <f>SUM(D7:D701)</f>
         <v>7.8649603525142539E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="9">
+        <f>_xlfn.T.DIST.RT(G4,1000)</f>
+        <v>7.8805232066711861E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -448,7 +543,7 @@
         <v>7.6995126189534227E-39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>A7+0.1</f>
         <v>0.1</v>
@@ -466,7 +561,7 @@
         <v>2.7615629744274633E-37</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ref="A9:A72" si="3">A8+0.1</f>
         <v>0.2</v>
@@ -484,7 +579,7 @@
         <v>9.1468931704346908E-36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
@@ -502,7 +597,7 @@
         <v>2.797859879441941E-34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="3"/>
         <v>0.4</v>
@@ -520,7 +615,7 @@
         <v>7.9034948269272958E-33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="3"/>
         <v>0.5</v>
@@ -538,7 +633,7 @@
         <v>2.0618679089020272E-31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="3"/>
         <v>0.6</v>
@@ -556,7 +651,7 @@
         <v>4.9677418697586477E-30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="3"/>
         <v>0.7</v>
@@ -574,7 +669,7 @@
         <v>1.1054072005252739E-28</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="3"/>
         <v>0.79999999999999993</v>
@@ -592,7 +687,7 @@
         <v>2.2717459503183183E-27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="3"/>
         <v>0.89999999999999991</v>

</xml_diff>